<commit_message>
build maps and updated BOMs
</commit_message>
<xml_diff>
--- a/hardware/TELEXi/board/TELEXi-BOM.xlsx
+++ b/hardware/TELEXi/board/TELEXi-BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14100" yWindow="2560" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="2560" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TELEXi" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Telex_I" localSheetId="0">TELEXi!$A$1:$H$22</definedName>
+    <definedName name="Telex_I_1" localSheetId="0">TELEXi!$A$1:$I$22</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="96">
   <si>
     <t>Qty</t>
   </si>
@@ -70,12 +70,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Parts</t>
-  </si>
-  <si>
-    <t>MF</t>
-  </si>
-  <si>
     <t>OC_MOUSER</t>
   </si>
   <si>
@@ -106,9 +100,6 @@
     <t>1x14 Header</t>
   </si>
   <si>
-    <t>T-LEFT-F, T-LEFT-M, T-RIGHT-F, T-RIGHT-M</t>
-  </si>
-  <si>
     <t>MO3PTH</t>
   </si>
   <si>
@@ -121,9 +112,6 @@
     <t>1x3 Header</t>
   </si>
   <si>
-    <t>II1, II2</t>
-  </si>
-  <si>
     <t>M06SILK_FEMALE_PTH</t>
   </si>
   <si>
@@ -133,9 +121,6 @@
     <t>1x6 Header</t>
   </si>
   <si>
-    <t>S-LEFT-F, S-LEFT-M, S-RIGHT-F, S-RIGHT-M</t>
-  </si>
-  <si>
     <t>MP3x2POGO_PINS</t>
   </si>
   <si>
@@ -148,9 +133,6 @@
     <t>2x3 Header</t>
   </si>
   <si>
-    <t>ADDRESS</t>
-  </si>
-  <si>
     <t>MCP1703CB</t>
   </si>
   <si>
@@ -178,9 +160,6 @@
     <t>5x2 Europower</t>
   </si>
   <si>
-    <t>POWER</t>
-  </si>
-  <si>
     <t>ALPHA-9MMF2A</t>
   </si>
   <si>
@@ -190,9 +169,6 @@
     <t>B10K Pot</t>
   </si>
   <si>
-    <t>POT1, POT2, POT3, POT4</t>
-  </si>
-  <si>
     <t>.01u</t>
   </si>
   <si>
@@ -214,27 +190,18 @@
     <t>4,700p</t>
   </si>
   <si>
-    <t>C104, C106, C107, C108</t>
-  </si>
-  <si>
     <t>81-GRM1885C1H472JA1D</t>
   </si>
   <si>
     <t>.1u</t>
   </si>
   <si>
-    <t>C1, C2, C100, C101, C102, C103, C105, C112, C113, C114</t>
-  </si>
-  <si>
     <t>581-06033C104JAT2A</t>
   </si>
   <si>
     <t>1u</t>
   </si>
   <si>
-    <t>C4, C111, C115, C116</t>
-  </si>
-  <si>
     <t>581-06033C105KAT2A</t>
   </si>
   <si>
@@ -244,9 +211,6 @@
     <t>CAP1206</t>
   </si>
   <si>
-    <t>C109, C110</t>
-  </si>
-  <si>
     <t>81-GRM31CR71E106KA12</t>
   </si>
   <si>
@@ -259,12 +223,6 @@
     <t>Fuses</t>
   </si>
   <si>
-    <t>F100, F101</t>
-  </si>
-  <si>
-    <t>Littelfuse</t>
-  </si>
-  <si>
     <t>576-0805L010</t>
   </si>
   <si>
@@ -277,9 +235,6 @@
     <t>Kobiconn 3.5mm</t>
   </si>
   <si>
-    <t>CV1, CV2, CV3, CV4</t>
-  </si>
-  <si>
     <t>MCP6004</t>
   </si>
   <si>
@@ -295,9 +250,6 @@
     <t>IC101</t>
   </si>
   <si>
-    <t>Microshop</t>
-  </si>
-  <si>
     <t>579-MCP6004T-I/SL</t>
   </si>
   <si>
@@ -313,9 +265,6 @@
     <t>Resistor .1%</t>
   </si>
   <si>
-    <t>R100, R101, R102, R103, R107, R109, R111, R112</t>
-  </si>
-  <si>
     <t>667-ERA-3AEB204V</t>
   </si>
   <si>
@@ -343,9 +292,6 @@
     <t>D100</t>
   </si>
   <si>
-    <t>NXP</t>
-  </si>
-  <si>
     <t>771-BAS70-04-T/R</t>
   </si>
   <si>
@@ -355,7 +301,46 @@
     <t>Teensy 3.2</t>
   </si>
   <si>
-    <t>U$1</t>
+    <t>TopBottom</t>
+  </si>
+  <si>
+    <t>BottomTop</t>
+  </si>
+  <si>
+    <t>BottomBottom</t>
+  </si>
+  <si>
+    <t>C104,C106,C107,C108</t>
+  </si>
+  <si>
+    <t>C100, C101, C102, C103</t>
+  </si>
+  <si>
+    <t>C1,C2</t>
+  </si>
+  <si>
+    <t>C105,C112,C113,C114</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C111,C115,C116</t>
+  </si>
+  <si>
+    <t>C109,C110</t>
+  </si>
+  <si>
+    <t>F100,F101</t>
+  </si>
+  <si>
+    <t>R100,R101,R102,R103</t>
+  </si>
+  <si>
+    <t>R107,R109,R111,R112</t>
+  </si>
+  <si>
+    <t>1206-CAP</t>
   </si>
 </sst>
 </file>
@@ -419,7 +404,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
     <dxf>
       <font>
         <strike val="0"/>
@@ -434,24 +419,51 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
+        <color theme="1"/>
         <name val="Avenir Next Regular"/>
         <scheme val="none"/>
       </font>
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
+        <color theme="1"/>
+        <name val="Avenir Next Regular"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
         <name val="Avenir Next Regular"/>
         <scheme val="none"/>
       </font>
@@ -552,23 +564,24 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Telex-I" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Telex-I_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H22" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I22" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I22"/>
   <sortState ref="A2:J22">
     <sortCondition ref="E1:E22"/>
   </sortState>
-  <tableColumns count="8">
-    <tableColumn id="1" name="Qty" dataDxfId="7"/>
-    <tableColumn id="2" name="Value" dataDxfId="6"/>
-    <tableColumn id="3" name="Device" dataDxfId="5"/>
-    <tableColumn id="4" name="Package" dataDxfId="4"/>
-    <tableColumn id="5" name="Description" dataDxfId="3"/>
-    <tableColumn id="6" name="Parts" dataDxfId="2"/>
-    <tableColumn id="8" name="MF" dataDxfId="1"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Qty" dataDxfId="8"/>
+    <tableColumn id="2" name="Value" dataDxfId="7"/>
+    <tableColumn id="3" name="Device" dataDxfId="6"/>
+    <tableColumn id="4" name="Package" dataDxfId="5"/>
+    <tableColumn id="5" name="Description" dataDxfId="4"/>
+    <tableColumn id="12" name="TopBottom" dataDxfId="3"/>
+    <tableColumn id="14" name="BottomTop" dataDxfId="2"/>
+    <tableColumn id="9" name="BottomBottom" dataDxfId="1"/>
     <tableColumn id="10" name="OC_MOUSER" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -838,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,13 +864,14 @@
     <col min="3" max="3" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -874,411 +888,399 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1206</v>
+        <v>51</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>4</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -1286,65 +1288,59 @@
         <v>470</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated assembly frame, BOMs and TriggerOutput behavior for TR.M
</commit_message>
<xml_diff>
--- a/hardware/TELEXi/board/TELEXi-BOM.xlsx
+++ b/hardware/TELEXi/board/TELEXi-BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="2560" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="16680" yWindow="1220" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TELEXi" sheetId="1" r:id="rId1"/>
@@ -280,9 +280,6 @@
     <t>R104</t>
   </si>
   <si>
-    <t>71-TNPW0603470RBEEA</t>
-  </si>
-  <si>
     <t>BAS70-04</t>
   </si>
   <si>
@@ -341,6 +338,9 @@
   </si>
   <si>
     <t>1206-CAP</t>
+  </si>
+  <si>
+    <t>660-RN731JTTD4700B25</t>
   </si>
 </sst>
 </file>
@@ -854,7 +854,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,13 +888,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -1084,7 +1084,7 @@
         <v>41</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>45</v>
@@ -1107,13 +1107,13 @@
         <v>41</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>47</v>
@@ -1136,10 +1136,10 @@
         <v>41</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>49</v>
@@ -1156,13 +1156,13 @@
         <v>51</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>41</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>52</v>
@@ -1185,7 +1185,7 @@
         <v>55</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>56</v>
@@ -1248,10 +1248,10 @@
         <v>69</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>70</v>
@@ -1300,7 +1300,7 @@
         <v>74</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1308,22 +1308,22 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1331,16 +1331,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>